<commit_message>
Update test case and add scripts for Product Details.
</commit_message>
<xml_diff>
--- a/TestCases/SauceLabDemoTestCases.xlsx
+++ b/TestCases/SauceLabDemoTestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\SauceLabDemoCoverGo\TestCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98BFFCD4-81E1-41DA-823F-49387A565B08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDC63C2A-E0B5-4F5E-B1BA-9C43FB869198}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{E7F736EB-E3BA-4954-A2A9-8988FA40E944}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="75">
   <si>
     <t>Feature</t>
   </si>
@@ -278,6 +278,9 @@
   </si>
   <si>
     <t>The cart icon should be disabled</t>
+  </si>
+  <si>
+    <t>The Product Details page is loaded with the image, product description</t>
   </si>
 </sst>
 </file>
@@ -649,8 +652,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{303DC040-7036-4FEA-B35A-5BD886941185}">
   <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15:D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -747,7 +750,7 @@
       <c r="C6" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="4" t="s">
         <v>27</v>
       </c>
       <c r="E6" t="s">
@@ -763,6 +766,7 @@
     <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B7" s="3"/>
       <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
       <c r="E7" t="s">
         <v>31</v>
       </c>
@@ -776,6 +780,7 @@
     <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B8" s="3"/>
       <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
       <c r="E8" t="s">
         <v>32</v>
       </c>
@@ -789,6 +794,7 @@
     <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B9" s="3"/>
       <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
       <c r="E9" t="s">
         <v>33</v>
       </c>
@@ -819,7 +825,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
         <v>62</v>
       </c>
@@ -836,7 +842,7 @@
         <v>16</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>21</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1069,12 +1075,7 @@
       <c r="D32" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="19">
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="C6:C9"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="B15:B20"/>
-    <mergeCell ref="B21:B24"/>
+  <mergeCells count="20">
     <mergeCell ref="B25:B28"/>
     <mergeCell ref="D29:D32"/>
     <mergeCell ref="B2:B3"/>
@@ -1089,6 +1090,12 @@
     <mergeCell ref="D25:D28"/>
     <mergeCell ref="C25:C28"/>
     <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D6:D9"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="C6:C9"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="B15:B20"/>
+    <mergeCell ref="B21:B24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>